<commit_message>
fix/add pecha id to translation test file
</commit_message>
<xml_diff>
--- a/tests/pecha/parser/google_doc/translation/data/en/English Root text Translation Metadata.xlsx
+++ b/tests/pecha/parser/google_doc/translation/data/en/English Root text Translation Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tsundue\mycodes\toolkit-v2\tests\pecha\parser\google_doc\translation\data\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D82B2D8-8DED-45FE-927F-D5161D1D1293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E2AACC-77A8-4678-847B-FB232C292E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Entries</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>translation_of</t>
+  </si>
+  <si>
+    <t>IB66C26FB</t>
   </si>
 </sst>
 </file>
@@ -575,8 +578,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1023,7 +1026,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>

</xml_diff>